<commit_message>
Updated the boost converter PCB and buy list.
PCB updated to include Reference designators and hole sizes have been
fitted properly to the components.  Buy list was updated so that parts
with the same number are not listed twice.
</commit_message>
<xml_diff>
--- a/Things to buy as of 2-19-2014.xlsx
+++ b/Things to buy as of 2-19-2014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="286" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="582" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>Mouser.com Part Number</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Reference Designator</t>
   </si>
   <si>
-    <t>828-OP906 </t>
+    <t>828-OP906</t>
   </si>
   <si>
     <t>IR laser detector photodiode</t>
@@ -62,7 +62,7 @@
     <t>R2</t>
   </si>
   <si>
-    <t>513-NJM12904D </t>
+    <t>513-NJM12904D</t>
   </si>
   <si>
     <t>Op-amp comparator</t>
@@ -71,7 +71,7 @@
     <t>U1</t>
   </si>
   <si>
-    <t>571-1977477-2 </t>
+    <t>571-1977477-2</t>
   </si>
   <si>
     <t>Terminal block, 2 position</t>
@@ -80,7 +80,7 @@
     <t>TB1, TB2</t>
   </si>
   <si>
-    <t>859-LTL-1CHAE </t>
+    <t>859-LTL-1CHAE</t>
   </si>
   <si>
     <t>Activity indicator LED</t>
@@ -89,7 +89,7 @@
     <t>D2</t>
   </si>
   <si>
-    <t>660-MF1/4DCT52R2000F </t>
+    <t>660-MF1/4DCT52R2000F</t>
   </si>
   <si>
     <t>LED current limiter, 200 Ohms</t>
@@ -98,7 +98,7 @@
     <t>R3</t>
   </si>
   <si>
-    <t>810-FK14X7R1H105K </t>
+    <t>810-FK14X7R1H105K</t>
   </si>
   <si>
     <t>Bypass cap for op-amps, 1 uF</t>
@@ -107,7 +107,7 @@
     <t>C1</t>
   </si>
   <si>
-    <t>828-OPV310 </t>
+    <t>828-OPV310</t>
   </si>
   <si>
     <t>Laser diode</t>
@@ -116,15 +116,12 @@
     <t>D1</t>
   </si>
   <si>
-    <t>660-MF1/4DC1501F </t>
+    <t>660-MF1/4DC1501F</t>
   </si>
   <si>
     <t>Current limiting resistor, 1.5k Ohms</t>
   </si>
   <si>
-    <t>TB1</t>
-  </si>
-  <si>
     <t>CMF55500R00FEBF</t>
   </si>
   <si>
@@ -236,18 +233,12 @@
     <t>791-RC1/2-203JB</t>
   </si>
   <si>
-    <t>Bleeder resitor for leveling capacitor, 20 KOhm</t>
+    <t>Bleeder resistor for leveling capacitor, 20 KOhm</t>
   </si>
   <si>
     <t>R6</t>
   </si>
   <si>
-    <t>571-1977477-2</t>
-  </si>
-  <si>
-    <t>Terminal blocks for input and output</t>
-  </si>
-  <si>
     <t>517-4808-3000-CP</t>
   </si>
   <si>
@@ -258,9 +249,6 @@
   </si>
   <si>
     <t>Opto-isolator for H-Bridge interface</t>
-  </si>
-  <si>
-    <t>Input LED current limiter, 200 Ohms</t>
   </si>
   <si>
     <t>Pololu.com Part Number</t>
@@ -283,11 +271,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -309,18 +298,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -379,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,7 +366,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,15 +378,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,7 +390,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -445,10 +415,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -565,7 +535,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -575,18 +545,18 @@
         <v>1.37</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4" t="n">
         <f aca="false">C6*D6</f>
-        <v>5.48</v>
+        <v>10.96</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -607,7 +577,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -617,18 +587,18 @@
         <v>0.06</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" s="4" t="n">
         <f aca="false">C8*D8</f>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -670,7 +640,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -691,517 +661,454 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>18</v>
+      <c r="A13" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>1.37</v>
+        <v>0.25</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="4" t="n">
         <f aca="false">C13*D13</f>
-        <v>2.74</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>36</v>
+      <c r="A14" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D14" s="3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D14" s="7" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="4" t="n">
         <f aca="false">C14*D14</f>
-        <v>0.5</v>
+        <v>0.16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D15" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <f aca="false">C15*D15</f>
-        <v>0.16</v>
-      </c>
-      <c r="F15" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="n">
+        <f aca="false">C16*D16</f>
+        <v>0.44</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="10" t="n">
-        <v>0.44</v>
+        <v>41</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>0.23</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="8" t="n">
         <f aca="false">C17*D17</f>
-        <v>0.44</v>
+        <v>0.23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="10" t="n">
-        <v>0.23</v>
+        <v>43</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>1.06</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="E18" s="8" t="n">
         <f aca="false">C18*D18</f>
-        <v>0.23</v>
+        <v>1.06</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="10" t="n">
-        <v>1.06</v>
+        <v>45</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <v>0.61</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="10" t="n">
+      <c r="E19" s="8" t="n">
         <f aca="false">C19*D19</f>
-        <v>1.06</v>
+        <v>0.61</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="10" t="n">
-        <v>0.61</v>
+        <v>47</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <v>0.46</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="10" t="n">
+      <c r="E20" s="8" t="n">
         <f aca="false">C20*D20</f>
-        <v>0.61</v>
+        <v>0.46</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="10" t="n">
-        <v>0.46</v>
+        <v>49</v>
+      </c>
+      <c r="C21" s="8" t="n">
+        <v>4.64</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="8" t="n">
         <f aca="false">C21*D21</f>
-        <v>0.46</v>
+        <v>4.64</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="10" t="n">
-        <v>4.64</v>
+        <v>52</v>
+      </c>
+      <c r="C22" s="8" t="n">
+        <v>0.99</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="10" t="n">
+      <c r="E22" s="8" t="n">
         <f aca="false">C22*D22</f>
-        <v>4.64</v>
+        <v>0.99</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="10" t="n">
-        <v>0.99</v>
+        <v>54</v>
+      </c>
+      <c r="C23" s="8" t="n">
+        <v>0.88</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="10" t="n">
+      <c r="E23" s="8" t="n">
         <f aca="false">C23*D23</f>
-        <v>0.99</v>
+        <v>0.88</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="10" t="n">
-        <v>0.88</v>
+        <v>57</v>
+      </c>
+      <c r="C24" s="8" t="n">
+        <v>0.62</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="10" t="n">
+      <c r="E24" s="8" t="n">
         <f aca="false">C24*D24</f>
-        <v>0.88</v>
+        <v>0.62</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="10" t="n">
-        <v>0.62</v>
+        <v>60</v>
+      </c>
+      <c r="C25" s="8" t="n">
+        <v>0.19</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="E25" s="8" t="n">
         <f aca="false">C25*D25</f>
-        <v>0.62</v>
+        <v>0.19</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="10" t="n">
-        <v>0.19</v>
+        <v>63</v>
+      </c>
+      <c r="C26" s="8" t="n">
+        <v>0.52</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="8" t="n">
         <f aca="false">C26*D26</f>
-        <v>0.19</v>
+        <v>0.52</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="10" t="n">
-        <v>0.52</v>
+        <v>66</v>
+      </c>
+      <c r="C27" s="8" t="n">
+        <v>0.43</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="8" t="n">
         <f aca="false">C27*D27</f>
-        <v>0.52</v>
+        <v>0.43</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="10" t="n">
-        <v>0.43</v>
+        <v>69</v>
+      </c>
+      <c r="C28" s="8" t="n">
+        <v>0.49</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E28" s="10" t="n">
+      <c r="E28" s="8" t="n">
         <f aca="false">C28*D28</f>
-        <v>0.43</v>
+        <v>0.49</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="10" t="n">
-        <v>0.49</v>
+        <v>72</v>
+      </c>
+      <c r="C29" s="8" t="n">
+        <v>0.36</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="8" t="n">
         <f aca="false">C29*D29</f>
-        <v>0.49</v>
+        <v>0.36</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="10" t="n">
-        <v>0.36</v>
+        <v>75</v>
+      </c>
+      <c r="C30" s="8" t="n">
+        <v>0.28</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="8" t="n">
         <f aca="false">C30*D30</f>
-        <v>0.36</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="10" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E31" s="10" t="n">
-        <f aca="false">C31*D31</f>
-        <v>2.9</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>0.56</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="8" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="8" t="n">
+        <f aca="false">D32*C32</f>
+        <v>0.56</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="10" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E32" s="10" t="n">
-        <f aca="false">C32*D32</f>
-        <v>0.56</v>
-      </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>755</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C35" s="8" t="n">
+        <v>39.95</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8" t="n">
+        <f aca="false">C35*D35</f>
+        <v>39.95</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>1404</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="10" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E34" s="10" t="n">
-        <f aca="false">D34*C34</f>
-        <v>0.56</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="C36" s="8" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="8" t="n">
+        <f aca="false">D36*C36</f>
+        <v>1.7</v>
+      </c>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="4" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" s="4" t="n">
-        <f aca="false">C35*D35</f>
-        <v>0.12</v>
-      </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="n">
-        <v>755</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="10" t="n">
-        <v>39.95</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="10" t="n">
-        <f aca="false">C38*D38</f>
-        <v>39.95</v>
-      </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="n">
-        <v>1404</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="10" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E39" s="10" t="n">
-        <f aca="false">D39*C39</f>
-        <v>1.7</v>
-      </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" s="11" t="inlineStr">
-        <f aca="false">SUM(E1:E39)</f>
-        <is>
-          <t/>
-        </is>
+      <c r="E38" s="9" t="n">
+        <f aca="false">SUM(E1:E36)</f>
+        <v>94.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized the boost converter PCB and buy list.
</commit_message>
<xml_diff>
--- a/Things to buy as of 2-19-2014.xlsx
+++ b/Things to buy as of 2-19-2014.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>Mouser.com Part Number</t>
   </si>
@@ -200,7 +200,7 @@
     <t>Feedback voltage divider low side resistor, 1 MOhm</t>
   </si>
   <si>
-    <t>R4</t>
+    <t>R4, R6</t>
   </si>
   <si>
     <t>71-CMF5519M100GNBF</t>
@@ -228,15 +228,6 @@
   </si>
   <si>
     <t>POT1</t>
-  </si>
-  <si>
-    <t>791-RC1/2-203JB</t>
-  </si>
-  <si>
-    <t>Bleeder resistor for leveling capacitor, 20 KOhm</t>
-  </si>
-  <si>
-    <t>R6</t>
   </si>
   <si>
     <t>517-4808-3000-CP</t>
@@ -415,10 +406,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -618,6 +609,7 @@
         <v>29</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>30</v>
@@ -891,7 +883,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>59</v>
       </c>
@@ -902,11 +894,11 @@
         <v>0.19</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="8" t="n">
         <f aca="false">C25*D25</f>
-        <v>0.19</v>
+        <v>0.38</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>61</v>
@@ -975,7 +967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
@@ -983,132 +975,111 @@
         <v>72</v>
       </c>
       <c r="C29" s="8" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="8" t="n">
         <f aca="false">C29*D29</f>
-        <v>0.36</v>
-      </c>
-      <c r="F29" s="2" t="s">
+        <v>0.56</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C31" s="8" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="8" t="n">
+        <f aca="false">D31*C31</f>
+        <v>0.56</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="8" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" s="8" t="n">
-        <f aca="false">C30*D30</f>
-        <v>0.56</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>755</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="8" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E32" s="8" t="n">
-        <f aca="false">D32*C32</f>
-        <v>0.56</v>
-      </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C34" s="8" t="n">
+        <v>39.95</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8" t="n">
+        <f aca="false">C34*D34</f>
+        <v>39.95</v>
+      </c>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>755</v>
+        <v>1404</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" s="8" t="n">
-        <v>39.95</v>
+        <v>0.85</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="8" t="n">
-        <f aca="false">C35*D35</f>
-        <v>39.95</v>
+        <f aca="false">D35*C35</f>
+        <v>1.7</v>
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="n">
-        <v>1404</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="8" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E36" s="8" t="n">
-        <f aca="false">D36*C36</f>
-        <v>1.7</v>
-      </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="9" t="n">
-        <f aca="false">SUM(E1:E36)</f>
-        <v>94.15</v>
+    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="9" t="n">
+        <f aca="false">SUM(E1:E35)</f>
+        <v>93.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated parts list and boost converter PCB
</commit_message>
<xml_diff>
--- a/Things to buy as of 2-19-2014.xlsx
+++ b/Things to buy as of 2-19-2014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="582" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="945" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>Mouser.com Part Number</t>
   </si>
@@ -155,7 +155,7 @@
     <t>R2 timing resistor for 555 Timer, 40 KOhm</t>
   </si>
   <si>
-    <t>71-CMF6080R000BHEB</t>
+    <t>71-RS00280R00FE70</t>
   </si>
   <si>
     <t>Output current limiting resistor for 555 Timer, 80 Ohm</t>
@@ -194,22 +194,31 @@
     <t>C2</t>
   </si>
   <si>
+    <t>660-MF1/4DCT52R9532F</t>
+  </si>
+  <si>
+    <t>Feedback voltage divider high side resistor, 95.3 kOhm</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>71-CMF555K0000BHEB</t>
+  </si>
+  <si>
+    <t>Feedback voltage divider low side resistor, 5.0 kOhm</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
     <t>594-VR37000001004FR5</t>
   </si>
   <si>
-    <t>Feedback voltage divider low side resistor, 1 MOhm</t>
-  </si>
-  <si>
-    <t>R4, R6</t>
-  </si>
-  <si>
-    <t>71-CMF5519M100GNBF</t>
-  </si>
-  <si>
-    <t>Feedback voltage divider high side resistor, 19.1 MOhm</t>
-  </si>
-  <si>
-    <t>R5</t>
+    <t>Output capacitor bleeder resistor, 1 Mohm</t>
+  </si>
+  <si>
+    <t>R6</t>
   </si>
   <si>
     <t>595-RC4558P</t>
@@ -406,10 +415,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -778,7 +787,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -891,20 +900,20 @@
         <v>60</v>
       </c>
       <c r="C25" s="8" t="n">
-        <v>0.19</v>
+        <v>0.06</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="8" t="n">
-        <f aca="false">C25*D25</f>
-        <v>0.38</v>
+        <f aca="false">D25*C25</f>
+        <v>0.06</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -912,20 +921,20 @@
         <v>63</v>
       </c>
       <c r="C26" s="8" t="n">
-        <v>0.52</v>
+        <v>0.59</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E26" s="8" t="n">
-        <f aca="false">C26*D26</f>
-        <v>0.52</v>
+        <f aca="false">D26*C26</f>
+        <v>0.59</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
@@ -933,14 +942,14 @@
         <v>66</v>
       </c>
       <c r="C27" s="8" t="n">
-        <v>0.43</v>
+        <v>0.19</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="8" t="n">
         <f aca="false">C27*D27</f>
-        <v>0.43</v>
+        <v>0.19</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>67</v>
@@ -954,14 +963,14 @@
         <v>69</v>
       </c>
       <c r="C28" s="8" t="n">
-        <v>0.49</v>
+        <v>0.43</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="8" t="n">
         <f aca="false">C28*D28</f>
-        <v>0.49</v>
+        <v>0.43</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>70</v>
@@ -975,111 +984,132 @@
         <v>72</v>
       </c>
       <c r="C29" s="8" t="n">
-        <v>0.28</v>
+        <v>0.49</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="8" t="n">
         <f aca="false">C29*D29</f>
+        <v>0.49</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="8" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="8" t="n">
+        <f aca="false">C30*D30</f>
         <v>0.56</v>
       </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="8"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="8" t="n">
+    <row r="31" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="8" t="n">
         <v>0.28</v>
       </c>
-      <c r="D31" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E31" s="8" t="n">
-        <f aca="false">D31*C31</f>
+      <c r="D32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="8" t="n">
+        <f aca="false">D32*C32</f>
         <v>0.56</v>
       </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="n">
-        <v>755</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="8" t="n">
-        <v>39.95</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="8" t="n">
-        <f aca="false">C34*D34</f>
-        <v>39.95</v>
-      </c>
-      <c r="F34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
+        <v>755</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="8" t="n">
+        <v>39.95</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8" t="n">
+        <f aca="false">C35*D35</f>
+        <v>39.95</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
         <v>1404</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="8" t="n">
+      <c r="B36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="8" t="n">
         <v>0.85</v>
       </c>
-      <c r="D35" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" s="8" t="n">
-        <f aca="false">D35*C35</f>
+      <c r="D36" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="8" t="n">
+        <f aca="false">D36*C36</f>
         <v>1.7</v>
       </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="9" t="n">
-        <f aca="false">SUM(E1:E35)</f>
-        <v>93.98</v>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="9" t="n">
+        <f aca="false">SUM(E1:E36)</f>
+        <v>93.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>